<commit_message>
Data Images and Data review map
</commit_message>
<xml_diff>
--- a/matlab/Data_Conversion/Conv.xlsx
+++ b/matlab/Data_Conversion/Conv.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Github 2018\Lake-Erie-2019\matlab\Data Conversion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Github 2018\Lake-Erie-2019\matlab\Data_Conversion\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="62">
   <si>
     <t>ACIDITY</t>
   </si>
@@ -207,6 +207,9 @@
   </si>
   <si>
     <t>WQ_OGM_POP</t>
+  </si>
+  <si>
+    <t>WQ_DIAG_TOT_PAR</t>
   </si>
 </sst>
 </file>
@@ -557,7 +560,7 @@
   <dimension ref="A1:C40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -799,7 +802,7 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>19</v>
+        <v>61</v>
       </c>
       <c r="C21">
         <v>1</v>

</xml_diff>